<commit_message>
modified:   Voice And Text/data_dictionary.xlsx 	new file:   Voice And Text/myInterview.txt 	modified:   Voice And Text/wordSplit.py 	modified:   Voice And Text/word_change_dic.py 	deleted:    Voice And Text/myInterview.txt
</commit_message>
<xml_diff>
--- a/Voice And Text/data_dictionary.xlsx
+++ b/Voice And Text/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d5c4b88138005b1/바탕 화면/CapstonProject_2023_1/Voice And Text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{A8629684-EEDA-471B-8C94-CA9956A7A6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E44B5199-AC66-48E3-A2C5-BD138BC646B0}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A8629684-EEDA-471B-8C94-CA9956A7A6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EDEAD61-3B7C-4B98-AD6B-9BE915EA3EFF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01848044-77DD-4A2D-9356-9EE5584307CC}"/>
+    <workbookView xWindow="-25935" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{01848044-77DD-4A2D-9356-9EE5584307CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>데터베스</t>
+    <t>데이터베이스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터베이스</t>
+    <t>테 터베 스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>터베</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -111,6 +115,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,20 +418,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5181AE-E0BE-4094-BAA2-CBF6E4DA6175}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>